<commit_message>
Its costly to develop
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="65">
   <si>
     <t>Component Name</t>
   </si>
@@ -119,9 +119,6 @@
     <t>Connector 2x8</t>
   </si>
   <si>
-    <t>Connector 1x20</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
@@ -201,6 +198,27 @@
   </si>
   <si>
     <t>ESP-32 DEVKITC</t>
+  </si>
+  <si>
+    <t>KF301-2P</t>
+  </si>
+  <si>
+    <t>Connector 1x16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total = </t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Manufacture</t>
+  </si>
+  <si>
+    <t>Soldering</t>
+  </si>
+  <si>
+    <t>Soldering Station</t>
   </si>
 </sst>
 </file>
@@ -210,7 +228,7 @@
   <numFmts count="1">
     <numFmt numFmtId="6" formatCode="&quot;R&quot;\ #,##0;[Red]&quot;R&quot;\ \-#,##0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -233,8 +251,15 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +272,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -327,11 +357,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -342,32 +388,45 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="1" builtinId="10"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="4">
     <dxf>
-      <border outline="0">
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
       </border>
     </dxf>
     <dxf>
@@ -418,15 +477,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F43" totalsRowShown="0" headerRowDxfId="2" headerRowBorderDxfId="1" tableBorderDxfId="0">
-  <autoFilter ref="A1:F43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F45" totalsRowShown="0" headerRowDxfId="3" headerRowBorderDxfId="1" tableBorderDxfId="2">
+  <autoFilter ref="A1:F45"/>
   <tableColumns count="6">
     <tableColumn id="1" name="Component Name"/>
     <tableColumn id="2" name="Part Number"/>
     <tableColumn id="3" name="Description"/>
     <tableColumn id="6" name="Value"/>
     <tableColumn id="4" name="Supplier"/>
-    <tableColumn id="5" name="Price per unit (Rands)"/>
+    <tableColumn id="5" name="Price per unit (Rands)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight13" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -695,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F43"/>
+  <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -708,7 +767,7 @@
     <col min="3" max="3" width="18.85546875" customWidth="1"/>
     <col min="4" max="4" width="15.42578125" customWidth="1"/>
     <col min="5" max="5" width="22.42578125" customWidth="1"/>
-    <col min="6" max="6" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -721,13 +780,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>50</v>
+      <c r="D1" s="5" t="s">
+        <v>49</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
     </row>
@@ -736,13 +795,16 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
         <v>8</v>
+      </c>
+      <c r="F2" s="6">
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -750,13 +812,16 @@
         <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>6</v>
       </c>
       <c r="E3" t="s">
         <v>9</v>
+      </c>
+      <c r="F3" s="6">
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -764,13 +829,16 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C4" t="s">
         <v>12</v>
       </c>
       <c r="E4" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="F4" s="6">
+        <v>70</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -778,13 +846,16 @@
         <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C5" t="s">
         <v>19</v>
       </c>
       <c r="E5" t="s">
         <v>8</v>
+      </c>
+      <c r="F5" s="6">
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -792,7 +863,7 @@
         <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C6" t="s">
         <v>19</v>
@@ -806,7 +877,7 @@
         <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C7" t="s">
         <v>19</v>
@@ -820,7 +891,7 @@
         <v>16</v>
       </c>
       <c r="B8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C8" t="s">
         <v>19</v>
@@ -853,7 +924,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
@@ -866,17 +937,26 @@
       <c r="A12" t="s">
         <v>21</v>
       </c>
+      <c r="B12" t="s">
+        <v>58</v>
+      </c>
       <c r="C12" t="s">
         <v>28</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
+      </c>
+      <c r="F12" s="6">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>22</v>
       </c>
+      <c r="B13" t="s">
+        <v>58</v>
+      </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
@@ -888,6 +968,9 @@
       <c r="A14" t="s">
         <v>23</v>
       </c>
+      <c r="B14" t="s">
+        <v>58</v>
+      </c>
       <c r="C14" t="s">
         <v>28</v>
       </c>
@@ -900,7 +983,7 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E15" t="s">
         <v>8</v>
@@ -911,16 +994,19 @@
         <v>25</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>26</v>
       </c>
+      <c r="B17" t="s">
+        <v>58</v>
+      </c>
       <c r="C17" t="s">
         <v>29</v>
       </c>
@@ -928,10 +1014,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>27</v>
       </c>
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
       <c r="C18" t="s">
         <v>30</v>
       </c>
@@ -939,288 +1028,334 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="E19" t="s">
+        <v>8</v>
+      </c>
+      <c r="F19" s="6">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>32</v>
       </c>
-      <c r="C19" t="s">
-        <v>40</v>
-      </c>
-      <c r="E19" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="C20" t="s">
+        <v>39</v>
+      </c>
+      <c r="E20" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>33</v>
       </c>
-      <c r="C20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="C21" t="s">
+        <v>39</v>
+      </c>
+      <c r="E21" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>34</v>
       </c>
-      <c r="C21" t="s">
-        <v>40</v>
-      </c>
-      <c r="E21" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="C22" t="s">
+        <v>39</v>
+      </c>
+      <c r="E22" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>35</v>
       </c>
-      <c r="C22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="C23" t="s">
+        <v>39</v>
+      </c>
+      <c r="E23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>36</v>
       </c>
-      <c r="C23" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E24" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>37</v>
       </c>
-      <c r="C24" t="s">
-        <v>40</v>
-      </c>
-      <c r="E24" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="E25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>38</v>
       </c>
-      <c r="C25" t="s">
-        <v>40</v>
-      </c>
-      <c r="E25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
         <v>39</v>
       </c>
-      <c r="C26" t="s">
-        <v>40</v>
-      </c>
       <c r="E26" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="5">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
         <v>1</v>
       </c>
       <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="E27" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="4">
+        <v>2</v>
+      </c>
+      <c r="C28" t="s">
+        <v>41</v>
+      </c>
+      <c r="E28" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>4</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="E30" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>5</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="E31" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>6</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="E32" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>7</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="E33" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>8</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="E34" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>9</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="E35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>10</v>
+      </c>
+      <c r="C36" t="s">
+        <v>41</v>
+      </c>
+      <c r="E36" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>11</v>
+      </c>
+      <c r="C37" t="s">
+        <v>41</v>
+      </c>
+      <c r="E37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="4">
+        <v>12</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="4">
+        <v>13</v>
+      </c>
+      <c r="C39" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>42</v>
       </c>
-      <c r="E27" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>42</v>
-      </c>
-      <c r="E28" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="5">
-        <v>3</v>
-      </c>
-      <c r="C29" t="s">
-        <v>42</v>
-      </c>
-      <c r="E29" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A30" s="5">
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>42</v>
-      </c>
-      <c r="E30" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="5">
-        <v>5</v>
-      </c>
-      <c r="C31" t="s">
-        <v>42</v>
-      </c>
-      <c r="E31" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5">
-        <v>6</v>
-      </c>
-      <c r="C32" t="s">
-        <v>42</v>
-      </c>
-      <c r="E32" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5">
-        <v>7</v>
-      </c>
-      <c r="C33" t="s">
-        <v>42</v>
-      </c>
-      <c r="E33" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
-        <v>8</v>
-      </c>
-      <c r="C34" t="s">
-        <v>42</v>
-      </c>
-      <c r="E34" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="5">
-        <v>9</v>
-      </c>
-      <c r="C35" t="s">
-        <v>42</v>
-      </c>
-      <c r="E35" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A36" s="5">
-        <v>10</v>
-      </c>
-      <c r="C36" t="s">
-        <v>42</v>
-      </c>
-      <c r="E36" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="5">
-        <v>11</v>
-      </c>
-      <c r="C37" t="s">
-        <v>42</v>
-      </c>
-      <c r="E37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5">
-        <v>12</v>
-      </c>
-      <c r="C38" t="s">
-        <v>42</v>
-      </c>
-      <c r="E38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5">
-        <v>13</v>
-      </c>
-      <c r="C39" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B40" t="s">
+        <v>55</v>
+      </c>
+      <c r="C40" t="s">
         <v>43</v>
       </c>
-      <c r="B40" t="s">
+      <c r="E40" t="s">
+        <v>8</v>
+      </c>
+      <c r="F40" s="6">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>44</v>
+      </c>
+      <c r="B41" t="s">
         <v>56</v>
       </c>
-      <c r="C40" t="s">
-        <v>44</v>
-      </c>
-      <c r="E40" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+      <c r="E41" t="s">
+        <v>8</v>
+      </c>
+      <c r="F41" s="6">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
         <v>45</v>
       </c>
-      <c r="B41" t="s">
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+      <c r="C42" t="s">
+        <v>46</v>
+      </c>
+      <c r="E42" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C43" t="s">
+        <v>64</v>
+      </c>
+      <c r="F43" s="6">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="C44" t="s">
+        <v>62</v>
+      </c>
+      <c r="F44" s="6">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" t="s">
         <v>57</v>
       </c>
-      <c r="C41" t="s">
-        <v>47</v>
-      </c>
-      <c r="E41" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>46</v>
-      </c>
-      <c r="B42" t="s">
-        <v>57</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
-      </c>
-      <c r="E42" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+      <c r="C45" t="s">
         <v>48</v>
       </c>
-      <c r="B43" t="s">
-        <v>58</v>
-      </c>
-      <c r="C43" t="s">
-        <v>49</v>
+      <c r="F45" s="6">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="E46" s="8" t="s">
+        <v>60</v>
+      </c>
+      <c r="F46" s="9">
+        <f>SUM(Table1[Price per unit (Rands)])</f>
+        <v>1719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>